<commit_message>
Add ability to support multiple entries per form
</commit_message>
<xml_diff>
--- a/app/assets/stylesheets/Steve Jobs (12).xlsx
+++ b/app/assets/stylesheets/Steve Jobs (12).xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -83,8 +83,35 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="28.389887640449437"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.989887640449439"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="28.389887640449437"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="28.389887640449437"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="4.189887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -148,6 +175,41 @@
           <t>q1_opt2</t>
         </is>
       </c>
+      <c r="M1" s="0" t="inlineStr">
+        <is>
+          <t>q1_opt3</t>
+        </is>
+      </c>
+      <c r="N1" s="0" t="inlineStr">
+        <is>
+          <t>q2_opt1</t>
+        </is>
+      </c>
+      <c r="O1" s="0" t="inlineStr">
+        <is>
+          <t>q2_opt2</t>
+        </is>
+      </c>
+      <c r="P1" s="0" t="inlineStr">
+        <is>
+          <t>q2_opt3</t>
+        </is>
+      </c>
+      <c r="Q1" s="0" t="inlineStr">
+        <is>
+          <t>q3_opt1</t>
+        </is>
+      </c>
+      <c r="R1" s="0" t="inlineStr">
+        <is>
+          <t>q3_opt2</t>
+        </is>
+      </c>
+      <c r="S1" s="0" t="inlineStr">
+        <is>
+          <t>q3_opt3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
@@ -200,12 +262,47 @@
       </c>
       <c r="K2" s="0" t="inlineStr">
         <is>
-          <t>Choice 1 yo</t>
+          <t>Choice 1</t>
         </is>
       </c>
       <c r="L2" s="0" t="inlineStr">
         <is>
-          <t>choice 2 boi</t>
+          <t>Choice 2</t>
+        </is>
+      </c>
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>Choice 3</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>Check 1</t>
+        </is>
+      </c>
+      <c r="O2" s="0" t="inlineStr">
+        <is>
+          <t>Check 2</t>
+        </is>
+      </c>
+      <c r="P2" s="0" t="inlineStr">
+        <is>
+          <t>Check 3</t>
+        </is>
+      </c>
+      <c r="Q2" s="0" t="inlineStr">
+        <is>
+          <t>Stressed out?</t>
+        </is>
+      </c>
+      <c r="R2" s="0" t="inlineStr">
+        <is>
+          <t>Relaxed?</t>
+        </is>
+      </c>
+      <c r="S2" s="0" t="inlineStr">
+        <is>
+          <t>In pain?</t>
         </is>
       </c>
     </row>
@@ -254,13 +351,94 @@
         </is>
       </c>
       <c r="J3" s="2">
-        <v>42707.95017637457</v>
+        <v>42707.962511499216</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T3" s="2">
+        <v>42707.97142585126</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>42708.016006341655</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -308,13 +486,88 @@
         </is>
       </c>
       <c r="J4" s="2">
-        <v>42707.9502089895</v>
+        <v>42707.96312438869</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="2">
+        <v>42707.97153375884</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>42708.01611987991</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM4" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>